<commit_message>
Times data OpenMP and remove write output
</commit_message>
<xml_diff>
--- a/taller 1/grafico.xlsx
+++ b/taller 1/grafico.xlsx
@@ -125,13 +125,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -10545,7 +10545,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14036,7 +14035,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14143,7 +14141,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14218,7 +14215,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -29803,7 +29799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D51" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D98" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="AO85" sqref="AO85"/>
     </sheetView>
   </sheetViews>
@@ -29823,28 +29819,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
       <c r="D1" s="7"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="M1" s="9" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="M1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -29860,15 +29856,15 @@
       <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
       <c r="N2" s="8" t="s">
         <v>0</v>
       </c>
@@ -29876,11 +29872,11 @@
         <v>2</v>
       </c>
       <c r="P2" s="12"/>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
     </row>
     <row r="3" spans="1:19" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">

</xml_diff>